<commit_message>
ALl cucumber projects add
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Firstname</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Mary</t>
   </si>
   <si>
-    <t>Brown</t>
-  </si>
-  <si>
     <t>PO</t>
   </si>
   <si>
@@ -58,20 +55,16 @@
     <t>Lee</t>
   </si>
   <si>
-    <t>SDET</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>Jones</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Jane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -398,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -416,64 +409,49 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="n">
-        <v>200000.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="n">
-        <v>110000.0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="n">
-        <v>135000.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="n">
-        <v>125000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>